<commit_message>
Ejercicios con Base de datos
</commit_message>
<xml_diff>
--- a/db_hospital.xlsx
+++ b/db_hospital.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xav-j12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FC2EEF0-350C-4256-ABB9-85C3E2CA4443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2B03EA-B54F-49F3-BFF5-FF37CFA388CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{96C65B63-FA5D-429C-A1F3-94D26BA5AEC0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{96C65B63-FA5D-429C-A1F3-94D26BA5AEC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hospital" sheetId="1" r:id="rId1"/>
+    <sheet name="estadisticas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="71">
   <si>
     <t>PACIENTE</t>
   </si>
@@ -220,6 +221,33 @@
   </si>
   <si>
     <t>GIOVANNY</t>
+  </si>
+  <si>
+    <t>CONTAR</t>
+  </si>
+  <si>
+    <t>PROMEDIO</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>SUMA</t>
+  </si>
+  <si>
+    <t>RANGO</t>
+  </si>
+  <si>
+    <t>A1:K35</t>
+  </si>
+  <si>
+    <t>Consulta</t>
+  </si>
+  <si>
+    <t>E1</t>
   </si>
 </sst>
 </file>
@@ -578,11 +606,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363A3A89-618A-42AA-9659-E5C231C362B4}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1810,7 +1850,127 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{427C2D7E-0C27-4850-BE7B-03732A034458}">
+      <formula1>0</formula1>
+      <formula2>125</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{68DE5A47-6E7D-4191-8B0A-486F24F73547}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4CD760-6740-4E33-90A6-9BF78E4DF061}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <f>DCOUNT(Hospital!A1:K35,Hospital!E1,B1:L2)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{CDC7BA58-5C7D-4CF7-95AF-A46057055805}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{33D7395F-18FC-4A34-A10D-D18B1C1FB0E0}">
+      <formula1>0</formula1>
+      <formula2>125</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ejemplo Coincidir y BuscarV
</commit_message>
<xml_diff>
--- a/db_hospital.xlsx
+++ b/db_hospital.xlsx
@@ -8,18 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xav-j12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89519044-903E-4ADE-8B96-0BB2D1EA0D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8219EBB4-FB4E-490C-B11C-3EAF9DB290FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{96C65B63-FA5D-429C-A1F3-94D26BA5AEC0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{96C65B63-FA5D-429C-A1F3-94D26BA5AEC0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Consultas" sheetId="1" r:id="rId1"/>
-    <sheet name="Sintomas" sheetId="3" r:id="rId2"/>
-    <sheet name="EPS" sheetId="4" r:id="rId3"/>
-    <sheet name="Diag." sheetId="5" r:id="rId4"/>
-    <sheet name="estadisticas" sheetId="2" r:id="rId5"/>
+    <sheet name="Hospital" sheetId="6" r:id="rId1"/>
+    <sheet name="Consultas" sheetId="1" r:id="rId2"/>
+    <sheet name="Sintomas" sheetId="3" r:id="rId3"/>
+    <sheet name="EPS" sheetId="4" r:id="rId4"/>
+    <sheet name="Diag." sheetId="5" r:id="rId5"/>
+    <sheet name="estadisticas" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="6" r:id="rId7"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="87">
   <si>
     <t>PACIENTE</t>
   </si>
@@ -278,6 +282,27 @@
   </si>
   <si>
     <t>N° SALA</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>(en blanco)</t>
+  </si>
+  <si>
+    <t>Total general</t>
+  </si>
+  <si>
+    <t>Etiquetas de columna</t>
+  </si>
+  <si>
+    <t>recaudado</t>
+  </si>
+  <si>
+    <t>Columna1</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -365,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -384,117 +409,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="51">
     <dxf>
       <font>
         <b val="0"/>
@@ -513,81 +442,9 @@
         <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -596,34 +453,8 @@
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
+        <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -648,6 +479,308 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1040,6 +1173,265 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="10" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
@@ -3967,17 +4359,789 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="EducacionIT" refreshedDate="44917.5755125" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="39" xr:uid="{DA49B621-9D02-4F27-BEBB-E37A76194E68}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="consultas"/>
+  </cacheSource>
+  <cacheFields count="11">
+    <cacheField name="PACIENTE" numFmtId="0">
+      <sharedItems containsBlank="1" count="35">
+        <s v="CARLOS"/>
+        <s v="ANDRES"/>
+        <s v="MARIA"/>
+        <s v="JUAN"/>
+        <s v="ROSA"/>
+        <s v="PEDRO"/>
+        <s v="ANA"/>
+        <s v="GLORIA"/>
+        <s v="JAIRO"/>
+        <s v="ONESIMO"/>
+        <s v="BERTHA"/>
+        <s v="BELKIS"/>
+        <s v="DORIS"/>
+        <s v="MARIO"/>
+        <s v="JAMES"/>
+        <s v="DAIRO"/>
+        <s v="DEIBER"/>
+        <s v="JULIA"/>
+        <s v="JORGE"/>
+        <s v="MARTHA"/>
+        <s v="DIANA"/>
+        <s v="NANCY"/>
+        <s v="YAMILE"/>
+        <s v="SAMIR"/>
+        <s v="JHON"/>
+        <s v="CINTIA"/>
+        <s v="SINDY"/>
+        <s v="ANAIS"/>
+        <s v="HENRY"/>
+        <s v="ALBERTO"/>
+        <s v="ALEX"/>
+        <s v="FREDY"/>
+        <s v="ISABEL"/>
+        <s v="GIOVANNY"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="FECHA ENTRADA" numFmtId="14">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2012-01-05T00:00:00" maxDate="2022-10-06T00:00:00"/>
+    </cacheField>
+    <cacheField name="SEXO" numFmtId="0">
+      <sharedItems containsBlank="1" count="3">
+        <s v="M"/>
+        <s v="F"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="EDAD" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="23" maxValue="60"/>
+    </cacheField>
+    <cacheField name="VALOR CONSULTA" numFmtId="6">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="25000" maxValue="75000"/>
+    </cacheField>
+    <cacheField name="SINTOMAS" numFmtId="0">
+      <sharedItems containsBlank="1" count="6">
+        <s v="DOLOR DE CABEZA"/>
+        <s v="MAREOS"/>
+        <s v="TOS"/>
+        <s v="DIARREA"/>
+        <s v="FIEBRE"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="EPS" numFmtId="0">
+      <sharedItems containsBlank="1" count="5">
+        <s v="SALUDCCOOP"/>
+        <s v="COOMEVA"/>
+        <s v="SALUDTOTAL"/>
+        <s v="NUEVA EPS"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="DIAGNOSTICO" numFmtId="0">
+      <sharedItems containsBlank="1" count="4">
+        <s v="GRIPE"/>
+        <s v="COLESTEROL ALTO"/>
+        <s v="PARASITOS"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="SALA" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="MEDICO" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Nº SALA" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="39">
+  <r>
+    <x v="0"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="0"/>
+    <n v="25"/>
+    <n v="25000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="102"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="0"/>
+    <n v="24"/>
+    <n v="45000"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="105"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="1"/>
+    <n v="28"/>
+    <n v="35000"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="104"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="0"/>
+    <n v="31"/>
+    <n v="25000"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="2"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="101"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="1"/>
+    <n v="35"/>
+    <n v="45000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="102"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="0"/>
+    <n v="45"/>
+    <n v="38000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="105"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="1"/>
+    <n v="23"/>
+    <n v="45000"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="104"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="1"/>
+    <n v="25"/>
+    <n v="75000"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="101"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="0"/>
+    <n v="28"/>
+    <n v="35000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="102"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="0"/>
+    <n v="29"/>
+    <n v="45000"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="105"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="1"/>
+    <n v="31"/>
+    <n v="35000"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="104"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="1"/>
+    <n v="45"/>
+    <n v="35000"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="101"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="1"/>
+    <n v="42"/>
+    <n v="25000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="102"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="0"/>
+    <n v="35"/>
+    <n v="45000"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="105"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="0"/>
+    <n v="42"/>
+    <n v="38000"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="104"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="0"/>
+    <n v="45"/>
+    <n v="45000"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="101"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="0"/>
+    <n v="35"/>
+    <n v="75000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="102"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="1"/>
+    <n v="36"/>
+    <n v="35000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="105"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="0"/>
+    <n v="25"/>
+    <n v="45000"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="104"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="1"/>
+    <n v="27"/>
+    <n v="35000"/>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="101"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="1"/>
+    <n v="28"/>
+    <n v="25000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="103"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="1"/>
+    <n v="23"/>
+    <n v="45000"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="104"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="1"/>
+    <n v="25"/>
+    <n v="75000"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="101"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="0"/>
+    <n v="28"/>
+    <n v="35000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="102"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="0"/>
+    <n v="29"/>
+    <n v="45000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="105"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="1"/>
+    <n v="31"/>
+    <n v="35000"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="104"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="1"/>
+    <n v="45"/>
+    <n v="35000"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="101"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="1"/>
+    <n v="42"/>
+    <n v="25000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="102"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="0"/>
+    <n v="35"/>
+    <n v="45000"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="105"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="0"/>
+    <n v="42"/>
+    <n v="38000"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="104"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="0"/>
+    <n v="45"/>
+    <n v="45000"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="101"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <d v="2012-02-05T00:00:00"/>
+    <x v="0"/>
+    <n v="35"/>
+    <n v="75000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="UCI"/>
+    <s v="PEDRO"/>
+    <n v="102"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="1"/>
+    <n v="36"/>
+    <n v="35000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="GENERAL"/>
+    <s v="MARIA"/>
+    <n v="105"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <d v="2012-01-05T00:00:00"/>
+    <x v="0"/>
+    <n v="25"/>
+    <n v="45000"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="URGENCIAS"/>
+    <s v="JUAN"/>
+    <n v="104"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <d v="2022-09-06T00:00:00"/>
+    <x v="0"/>
+    <n v="45"/>
+    <n v="25000"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="URGENCIAS"/>
+    <s v="MARIA"/>
+    <n v="102"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <d v="2022-10-05T00:00:00"/>
+    <x v="1"/>
+    <n v="60"/>
+    <n v="35000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="GENERAL"/>
+    <s v="PEDRO"/>
+    <n v="103"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="34"/>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="34"/>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A5859F3A-3B57-450A-9A70-00C5DCFE3F75}" name="TablaDinámica1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="36">
+        <item sd="0" x="29"/>
+        <item sd="0" x="30"/>
+        <item sd="0" x="6"/>
+        <item x="27"/>
+        <item x="1"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="0"/>
+        <item x="25"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="20"/>
+        <item x="12"/>
+        <item x="31"/>
+        <item x="33"/>
+        <item x="7"/>
+        <item x="28"/>
+        <item x="32"/>
+        <item x="8"/>
+        <item x="14"/>
+        <item x="24"/>
+        <item x="18"/>
+        <item x="3"/>
+        <item x="17"/>
+        <item x="2"/>
+        <item x="13"/>
+        <item x="19"/>
+        <item x="21"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="23"/>
+        <item x="26"/>
+        <item x="22"/>
+        <item x="34"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item sd="0" x="1"/>
+        <item sd="0" x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="7">
+        <item sd="0" x="3"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="6">
+        <item sd="0" x="1"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item sd="0" x="1"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="7"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="34"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="6"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="recaudado" fld="4" baseField="0" baseItem="9" numFmtId="44"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E441EFC-D1E8-4F6E-9C94-A3F8C6776698}" name="consultas" displayName="consultas" ref="A1:K40">
-  <autoFilter ref="A1:K40" xr:uid="{6E441EFC-D1E8-4F6E-9C94-A3F8C6776698}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E441EFC-D1E8-4F6E-9C94-A3F8C6776698}" name="consultas" displayName="consultas" ref="A1:L40">
+  <autoFilter ref="A1:L40" xr:uid="{6E441EFC-D1E8-4F6E-9C94-A3F8C6776698}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{EC82EA36-EB1F-49DB-A78A-F50AC33EE756}" name="PACIENTE" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{C8C2C046-88FD-4CEF-BF85-DB92A181E0F5}" name="FECHA ENTRADA" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{C8C2C046-88FD-4CEF-BF85-DB92A181E0F5}" name="FECHA ENTRADA" dataDxfId="50"/>
     <tableColumn id="3" xr3:uid="{ADD20D36-BD44-44DC-AD63-8C9CB8E591A8}" name="SEXO"/>
     <tableColumn id="4" xr3:uid="{10727B86-F67A-4CA2-89E7-579B6DE2B962}" name="EDAD"/>
-    <tableColumn id="5" xr3:uid="{188E4BC3-9DE6-4BEA-BA07-B0330A9C93BC}" name="VALOR CONSULTA" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{188E4BC3-9DE6-4BEA-BA07-B0330A9C93BC}" name="VALOR CONSULTA" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48"/>
     <tableColumn id="6" xr3:uid="{CE3245D0-4345-44E2-90AF-6B2883BC986D}" name="SINTOMAS"/>
     <tableColumn id="7" xr3:uid="{3805ABBF-FA67-4E8E-8032-9FCB8BF93218}" name="EPS"/>
+    <tableColumn id="12" xr3:uid="{0068C1F7-A36A-4CCC-89F9-E7D215E5FC0F}" name="P" dataDxfId="12">
+      <calculatedColumnFormula>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="8" xr3:uid="{5FF9DCF8-C812-4517-9BEA-20F822FA3431}" name="DIAGNOSTICO"/>
     <tableColumn id="9" xr3:uid="{6A64243D-9D68-40FF-BFC4-64EC77D0EC33}" name="SALA"/>
     <tableColumn id="10" xr3:uid="{7B5E8CF0-A178-4CD4-BE64-1CB1FE201BCC}" name="MEDICO"/>
@@ -3988,14 +5152,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C8448426-7384-4C17-9436-DBD879A4F2CB}" name="sala_nombres" displayName="sala_nombres" ref="M1:P5" totalsRowCount="1">
-  <autoFilter ref="M1:P4" xr:uid="{C8448426-7384-4C17-9436-DBD879A4F2CB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C8448426-7384-4C17-9436-DBD879A4F2CB}" name="sala_nombres" displayName="sala_nombres" ref="N1:Q5" totalsRowCount="1">
+  <autoFilter ref="N1:Q4" xr:uid="{C8448426-7384-4C17-9436-DBD879A4F2CB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9A4E74E3-608A-4BEA-BED4-7AD6FA092E4D}" name="SALA" totalsRowLabel="Total"/>
     <tableColumn id="3" xr3:uid="{FACAF06C-F4FD-4799-A2CB-6A45AA4B1799}" name="M" totalsRowFunction="sum"/>
     <tableColumn id="4" xr3:uid="{93C25959-9B38-45C7-B858-162B68C50D9F}" name="F" totalsRowFunction="sum"/>
     <tableColumn id="2" xr3:uid="{E14355DF-19BC-445F-95E0-15BA64BA38C3}" name="Total" totalsRowFunction="sum">
-      <calculatedColumnFormula>COUNTIF(consultas[SALA],M2)</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTIF(consultas[SALA],N2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4003,18 +5167,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{944FFD16-F8E9-4AB3-BC8B-54439875215D}" name="sala_numeros" displayName="sala_numeros" ref="M7:P14" totalsRowCount="1">
-  <autoFilter ref="M7:P13" xr:uid="{944FFD16-F8E9-4AB3-BC8B-54439875215D}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{944FFD16-F8E9-4AB3-BC8B-54439875215D}" name="sala_numeros" displayName="sala_numeros" ref="N7:R13" totalsRowCount="1">
+  <autoFilter ref="N7:R12" xr:uid="{944FFD16-F8E9-4AB3-BC8B-54439875215D}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F02196C5-358E-43B0-AC91-5CFCD0BD54B5}" name="N° SALA" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{3287619F-FF33-4119-9C3A-2BA196659CDB}" name="M" totalsRowFunction="sum" dataDxfId="7">
-      <calculatedColumnFormula>COUNTIFS(consultas[Nº SALA],$M8,consultas[SEXO],N$1)</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{3287619F-FF33-4119-9C3A-2BA196659CDB}" name="M" totalsRowFunction="sum" dataDxfId="47">
+      <calculatedColumnFormula>COUNTIFS(consultas[Nº SALA],$N8,consultas[SEXO],O$1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{71C9643A-8015-49E5-93EF-F0993CCE7A0B}" name="F" totalsRowFunction="sum" dataDxfId="6">
-      <calculatedColumnFormula>COUNTIFS(consultas[Nº SALA],$M8,consultas[SEXO],O$1)</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{71C9643A-8015-49E5-93EF-F0993CCE7A0B}" name="F" totalsRowFunction="sum" dataDxfId="46">
+      <calculatedColumnFormula>COUNTIFS(consultas[Nº SALA],$N8,consultas[SEXO],P$1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C61461CC-35A1-49D4-B2DB-3BDB6B07A3C3}" name="Total" totalsRowFunction="sum" dataDxfId="5">
-      <calculatedColumnFormula>COUNTIF(consultas[Nº SALA],M8)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{C61461CC-35A1-49D4-B2DB-3BDB6B07A3C3}" name="Total" totalsRowFunction="sum" dataDxfId="45">
+      <calculatedColumnFormula>COUNTIF(consultas[Nº SALA],N8)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{46FCE4AB-DE07-4B34-998E-864891C32607}" name="Columna1" dataDxfId="11">
+      <calculatedColumnFormula>MATCH(sala_numeros[[#This Row],[N° SALA]],consultas[Nº SALA],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4022,17 +5189,17 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1BD8535B-95FE-40ED-80F1-F867E2BB12CE}" name="sintomas" displayName="sintomas" ref="A1:D8" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1BD8535B-95FE-40ED-80F1-F867E2BB12CE}" name="sintomas" displayName="sintomas" ref="A1:D8" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A1:D7" xr:uid="{1BD8535B-95FE-40ED-80F1-F867E2BB12CE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FE59E412-D13D-4FFB-AC98-6B40A0D50C7E}" name="nombre" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{B40697AB-D92C-41F4-93FB-88A3DC66EE2C}" name="M" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="13">
+    <tableColumn id="1" xr3:uid="{FE59E412-D13D-4FFB-AC98-6B40A0D50C7E}" name="nombre" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{B40697AB-D92C-41F4-93FB-88A3DC66EE2C}" name="M" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39">
       <calculatedColumnFormula>COUNTIFS(consultas[SINTOMAS],sintomas[[#This Row],[nombre]],consultas[SEXO],sintomas[[#Headers],[M]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E2CC96D7-2DA9-4C89-8E37-CA0AA4C1F54B}" name="F" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="12">
+    <tableColumn id="4" xr3:uid="{E2CC96D7-2DA9-4C89-8E37-CA0AA4C1F54B}" name="F" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37">
       <calculatedColumnFormula>COUNTIFS(consultas[SINTOMAS],sintomas[[#This Row],[nombre]],consultas[SEXO],sintomas[[#Headers],[F]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7C946B64-55CF-46E8-83D7-95E10D913968}" name="cant" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="11">
+    <tableColumn id="2" xr3:uid="{7C946B64-55CF-46E8-83D7-95E10D913968}" name="cant" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35">
       <calculatedColumnFormula>COUNTIF(consultas[SINTOMAS],A2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4045,13 +5212,13 @@
   <autoFilter ref="A1:D5" xr:uid="{7688E62D-3E39-41D3-9434-2A47DCDDBFA5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B0AA9F69-BE41-42E4-97D5-421616661BC9}" name="nombre" totalsRowLabel="Total"/>
-    <tableColumn id="4" xr3:uid="{C3316FC6-E38D-47BD-967B-920AC817EA02}" name="M" totalsRowFunction="sum" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{C3316FC6-E38D-47BD-967B-920AC817EA02}" name="M" totalsRowFunction="sum" dataDxfId="34">
       <calculatedColumnFormula>COUNTIFS(consultas[EPS],eps[[#This Row],[nombre]],consultas[SEXO],eps[[#Headers],[M]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{74F84E4D-37F2-4F2C-A6A4-4D7382A164F4}" name="F" totalsRowFunction="sum" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{74F84E4D-37F2-4F2C-A6A4-4D7382A164F4}" name="F" totalsRowFunction="sum" dataDxfId="33">
       <calculatedColumnFormula>COUNTIFS(consultas[EPS],eps[[#This Row],[nombre]],consultas[SEXO],eps[[#Headers],[F]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{58C7F580-DE5E-47E5-A261-6E465FD82430}" name="cant" totalsRowFunction="sum" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{58C7F580-DE5E-47E5-A261-6E465FD82430}" name="cant" totalsRowFunction="sum" dataDxfId="32">
       <calculatedColumnFormula>COUNTIF(consultas[EPS],eps[[#This Row],[nombre]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4063,14 +5230,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{86F2E751-2B35-422B-8E7D-B1FF30734C49}" name="diagnostico" displayName="diagnostico" ref="A1:D5" totalsRowCount="1">
   <autoFilter ref="A1:D4" xr:uid="{86F2E751-2B35-422B-8E7D-B1FF30734C49}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8096F61C-2C59-4592-A42F-61BF15553F5D}" name="nombre" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{69922583-5ADD-4609-8A13-F309F9BF2617}" name="M" totalsRowFunction="sum" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{8096F61C-2C59-4592-A42F-61BF15553F5D}" name="nombre" totalsRowLabel="Total" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{69922583-5ADD-4609-8A13-F309F9BF2617}" name="M" totalsRowFunction="sum" dataDxfId="29">
       <calculatedColumnFormula>COUNTIFS(consultas[DIAGNOSTICO],diagnostico[[#This Row],[nombre]],consultas[SEXO],diagnostico[[#Headers],[M]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2E9574B2-FEDF-4473-B1B2-5F7BED59E396}" name="F" totalsRowFunction="sum" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{2E9574B2-FEDF-4473-B1B2-5F7BED59E396}" name="F" totalsRowFunction="sum" dataDxfId="28">
       <calculatedColumnFormula>COUNTIFS(consultas[DIAGNOSTICO],diagnostico[[#This Row],[nombre]],consultas[SEXO],diagnostico[[#Headers],[F]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{16E9E940-42D4-48C2-B17E-0511625B0478}" name="cant" totalsRowFunction="sum" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{16E9E940-42D4-48C2-B17E-0511625B0478}" name="cant" totalsRowFunction="sum" dataDxfId="27">
       <calculatedColumnFormula>COUNTIF(consultas[DIAGNOSTICO],diagnostico[[#This Row],[nombre]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4079,20 +5246,42 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{981CC706-1D39-4161-B333-B24C4E334487}" name="condiciones" displayName="condiciones" ref="A1:K2" totalsRowShown="0" headerRowDxfId="21" dataDxfId="22" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{981CC706-1D39-4161-B333-B24C4E334487}" name="condiciones" displayName="condiciones" ref="A1:K3" totalsRowCount="1" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
   <autoFilter ref="A1:K2" xr:uid="{981CC706-1D39-4161-B333-B24C4E334487}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{01AE878A-DBC7-4557-BBD6-D5D55A909672}" name="PACIENTE" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{C2EADEEC-4AEC-4D0B-A67B-BCF56FC6F7E6}" name="FECHA ENTRADA" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{FE98B3F5-EF62-48B9-8AAC-07870ABE0568}" name="SEXO" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{ED80729D-94D8-4AA7-89E5-C7F75FBD9D31}" name="EDAD" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{D21B0948-2F5B-4882-9A85-6079FA28F7D3}" name="VALOR CONSULTA" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{F07DB86B-840F-4A91-AF78-3EBE9FF94938}" name="SINTOMAS" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{8B97ECAE-C44A-4352-8245-F057FD32A5E1}" name="EPS" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{90E3307A-9018-4FE7-B90D-BFFDC7063DA2}" name="DIAGNOSTICO" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{3DB5A69B-1E06-4302-954C-896C7EB33553}" name="SALA" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{68459C48-FD1B-4091-BA0D-9F12ACE78A94}" name="MEDICO" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{E2F6BA46-1715-4664-B357-3382762F6E79}" name="Nº SALA" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{01AE878A-DBC7-4557-BBD6-D5D55A909672}" name="PACIENTE" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="10">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[PACIENTE]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{C2EADEEC-4AEC-4D0B-A67B-BCF56FC6F7E6}" name="FECHA ENTRADA" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="9">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[FECHA ENTRADA]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{FE98B3F5-EF62-48B9-8AAC-07870ABE0568}" name="SEXO" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="8">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[SEXO]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{ED80729D-94D8-4AA7-89E5-C7F75FBD9D31}" name="EDAD" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="7">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[EDAD]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{D21B0948-2F5B-4882-9A85-6079FA28F7D3}" name="VALOR CONSULTA" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="6">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[VALOR CONSULTA]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{F07DB86B-840F-4A91-AF78-3EBE9FF94938}" name="SINTOMAS" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="5">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[SINTOMAS]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{8B97ECAE-C44A-4352-8245-F057FD32A5E1}" name="EPS" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="4">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[EPS]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{90E3307A-9018-4FE7-B90D-BFFDC7063DA2}" name="DIAGNOSTICO" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="3">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[DIAGNOSTICO]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{3DB5A69B-1E06-4302-954C-896C7EB33553}" name="SALA" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="2">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[SALA]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{68459C48-FD1B-4091-BA0D-9F12ACE78A94}" name="MEDICO" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="1">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[MEDICO]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{E2F6BA46-1715-4664-B357-3382762F6E79}" name="Nº SALA" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="0">
+      <totalsRowFormula>MATCH(condiciones[[#Headers],[Nº SALA]],consultas[#Headers],0)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4394,11 +5583,194 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CF754D-FB60-4104-B35A-90837A53FE99}">
+  <dimension ref="A3:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="22">
+        <v>45000</v>
+      </c>
+      <c r="C5" s="22">
+        <v>70000</v>
+      </c>
+      <c r="D5" s="22">
+        <v>175000</v>
+      </c>
+      <c r="E5" s="22">
+        <v>90000</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22">
+        <v>380000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="22">
+        <v>198000</v>
+      </c>
+      <c r="C6" s="22">
+        <v>300000</v>
+      </c>
+      <c r="D6" s="22">
+        <v>155000</v>
+      </c>
+      <c r="E6" s="22">
+        <v>181000</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22">
+        <v>834000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="22">
+        <v>90000</v>
+      </c>
+      <c r="C7" s="22">
+        <v>25000</v>
+      </c>
+      <c r="D7" s="22">
+        <v>70000</v>
+      </c>
+      <c r="E7" s="22">
+        <v>90000</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22">
+        <v>275000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="22">
+        <v>333000</v>
+      </c>
+      <c r="C10" s="22">
+        <v>395000</v>
+      </c>
+      <c r="D10" s="22">
+        <v>400000</v>
+      </c>
+      <c r="E10" s="22">
+        <v>361000</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22">
+        <v>1489000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363A3A89-618A-42AA-9659-E5C231C362B4}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4410,15 +5782,17 @@
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="3.85546875" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4441,31 +5815,34 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4487,35 +5864,39 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>102</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="N2">
-        <f>COUNTIFS(consultas[SALA],$M2,consultas[SEXO],N$1)</f>
+      <c r="O2">
+        <f>COUNTIFS(consultas[SALA],$N2,consultas[SEXO],O$1)</f>
         <v>9</v>
       </c>
-      <c r="O2">
-        <f>COUNTIFS(consultas[SALA],$M2,consultas[SEXO],O$1)</f>
+      <c r="P2">
+        <f>COUNTIFS(consultas[SALA],$N2,consultas[SEXO],P$1)</f>
         <v>4</v>
       </c>
-      <c r="P2">
-        <f>COUNTIF(consultas[SALA],M2)</f>
+      <c r="Q2">
+        <f>COUNTIF(consultas[SALA],N2)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -4537,35 +5918,39 @@
       <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>23</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>105</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>22</v>
       </c>
-      <c r="N3">
-        <f>COUNTIFS(consultas[SALA],$M3,consultas[SEXO],N$1)</f>
+      <c r="O3">
+        <f>COUNTIFS(consultas[SALA],$N3,consultas[SEXO],O$1)</f>
         <v>5</v>
       </c>
-      <c r="O3">
-        <f>COUNTIFS(consultas[SALA],$M3,consultas[SEXO],O$1)</f>
+      <c r="P3">
+        <f>COUNTIFS(consultas[SALA],$N3,consultas[SEXO],P$1)</f>
         <v>6</v>
       </c>
-      <c r="P3">
-        <f>COUNTIF(consultas[SALA],M3)</f>
+      <c r="Q3">
+        <f>COUNTIF(consultas[SALA],N3)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -4587,35 +5972,39 @@
       <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>24</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>104</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>28</v>
       </c>
-      <c r="N4">
-        <f>COUNTIFS(consultas[SALA],$M4,consultas[SEXO],N$1)</f>
+      <c r="O4">
+        <f>COUNTIFS(consultas[SALA],$N4,consultas[SEXO],O$1)</f>
         <v>5</v>
       </c>
-      <c r="O4">
-        <f>COUNTIFS(consultas[SALA],$M4,consultas[SEXO],O$1)</f>
+      <c r="P4">
+        <f>COUNTIFS(consultas[SALA],$N4,consultas[SEXO],P$1)</f>
         <v>7</v>
       </c>
-      <c r="P4">
-        <f>COUNTIF(consultas[SALA],M4)</f>
+      <c r="Q4">
+        <f>COUNTIF(consultas[SALA],N4)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4637,35 +6026,39 @@
       <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
         <v>31</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>17</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>101</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>72</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <f>SUBTOTAL(109,sala_nombres[M])</f>
         <v>19</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <f>SUBTOTAL(109,sala_nombres[F])</f>
         <v>17</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <f>SUBTOTAL(109,sala_nombres[Total])</f>
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -4687,20 +6080,24 @@
       <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>22</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>23</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4722,32 +6119,39 @@
       <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>28</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>24</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>105</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>79</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>12</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>25</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>72</v>
       </c>
+      <c r="R7" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -4769,35 +6173,43 @@
       <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
         <v>21</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>16</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>17</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>104</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>101</v>
       </c>
-      <c r="N8">
-        <f>COUNTIFS(consultas[Nº SALA],$M8,consultas[SEXO],N$1)</f>
+      <c r="O8">
+        <f>COUNTIFS(consultas[Nº SALA],$N8,consultas[SEXO],O$1)</f>
         <v>3</v>
       </c>
-      <c r="O8">
-        <f>COUNTIFS(consultas[Nº SALA],$M8,consultas[SEXO],O$1)</f>
+      <c r="P8">
+        <f>COUNTIFS(consultas[Nº SALA],$N8,consultas[SEXO],P$1)</f>
         <v>5</v>
       </c>
-      <c r="P8">
-        <f>COUNTIF(consultas[Nº SALA],M8)</f>
+      <c r="Q8">
+        <f>COUNTIF(consultas[Nº SALA],N8)</f>
         <v>8</v>
       </c>
+      <c r="R8" s="20">
+        <f>MATCH(sala_numeros[[#This Row],[N° SALA]],consultas[Nº SALA],0)</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -4819,35 +6231,43 @@
       <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
         <v>15</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>22</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>23</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>101</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>102</v>
       </c>
-      <c r="N9">
-        <f>COUNTIFS(consultas[Nº SALA],$M9,consultas[SEXO],N$1)</f>
+      <c r="O9">
+        <f>COUNTIFS(consultas[Nº SALA],$N9,consultas[SEXO],O$1)</f>
         <v>6</v>
       </c>
-      <c r="O9">
-        <f>COUNTIFS(consultas[Nº SALA],$M9,consultas[SEXO],O$1)</f>
+      <c r="P9">
+        <f>COUNTIFS(consultas[Nº SALA],$N9,consultas[SEXO],P$1)</f>
         <v>3</v>
       </c>
-      <c r="P9">
-        <f>COUNTIF(consultas[Nº SALA],M9)</f>
+      <c r="Q9">
+        <f>COUNTIF(consultas[Nº SALA],N9)</f>
         <v>9</v>
       </c>
+      <c r="R9" s="20">
+        <f>MATCH(sala_numeros[[#This Row],[N° SALA]],consultas[Nº SALA],0)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -4869,35 +6289,43 @@
       <c r="G10" t="s">
         <v>14</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
         <v>31</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>28</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>24</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>102</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>103</v>
       </c>
-      <c r="N10">
-        <f>COUNTIFS(consultas[Nº SALA],$M10,consultas[SEXO],N$1)</f>
+      <c r="O10">
+        <f>COUNTIFS(consultas[Nº SALA],$N10,consultas[SEXO],O$1)</f>
         <v>0</v>
       </c>
-      <c r="O10">
-        <f>COUNTIFS(consultas[Nº SALA],$M10,consultas[SEXO],O$1)</f>
+      <c r="P10">
+        <f>COUNTIFS(consultas[Nº SALA],$N10,consultas[SEXO],P$1)</f>
         <v>2</v>
       </c>
-      <c r="P10">
-        <f>COUNTIF(consultas[Nº SALA],M10)</f>
+      <c r="Q10">
+        <f>COUNTIF(consultas[Nº SALA],N10)</f>
         <v>2</v>
       </c>
+      <c r="R10" s="20">
+        <f>MATCH(sala_numeros[[#This Row],[N° SALA]],consultas[Nº SALA],0)</f>
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -4919,35 +6347,43 @@
       <c r="G11" t="s">
         <v>20</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
         <v>15</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>16</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>17</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>105</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>104</v>
       </c>
-      <c r="N11">
-        <f>COUNTIFS(consultas[Nº SALA],$M11,consultas[SEXO],N$1)</f>
+      <c r="O11">
+        <f>COUNTIFS(consultas[Nº SALA],$N11,consultas[SEXO],O$1)</f>
         <v>4</v>
       </c>
-      <c r="O11">
-        <f>COUNTIFS(consultas[Nº SALA],$M11,consultas[SEXO],O$1)</f>
+      <c r="P11">
+        <f>COUNTIFS(consultas[Nº SALA],$N11,consultas[SEXO],P$1)</f>
         <v>5</v>
       </c>
-      <c r="P11">
-        <f>COUNTIF(consultas[Nº SALA],M11)</f>
+      <c r="Q11">
+        <f>COUNTIF(consultas[Nº SALA],N11)</f>
         <v>9</v>
       </c>
+      <c r="R11" s="20">
+        <f>MATCH(sala_numeros[[#This Row],[N° SALA]],consultas[Nº SALA],0)</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -4969,35 +6405,43 @@
       <c r="G12" t="s">
         <v>27</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
         <v>15</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>22</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>23</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>104</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>105</v>
       </c>
-      <c r="N12">
-        <f>COUNTIFS(consultas[Nº SALA],$M12,consultas[SEXO],N$1)</f>
+      <c r="O12">
+        <f>COUNTIFS(consultas[Nº SALA],$N12,consultas[SEXO],O$1)</f>
         <v>6</v>
       </c>
-      <c r="O12">
-        <f>COUNTIFS(consultas[Nº SALA],$M12,consultas[SEXO],O$1)</f>
+      <c r="P12">
+        <f>COUNTIFS(consultas[Nº SALA],$N12,consultas[SEXO],P$1)</f>
         <v>2</v>
       </c>
-      <c r="P12">
-        <f>COUNTIF(consultas[Nº SALA],M12)</f>
+      <c r="Q12">
+        <f>COUNTIF(consultas[Nº SALA],N12)</f>
         <v>8</v>
       </c>
+      <c r="R12" s="20">
+        <f>MATCH(sala_numeros[[#This Row],[N° SALA]],consultas[Nº SALA],0)</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -5019,35 +6463,39 @@
       <c r="G13" t="s">
         <v>30</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
         <v>21</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>28</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>24</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>101</v>
       </c>
-      <c r="M13">
-        <v>106</v>
-      </c>
-      <c r="N13">
-        <f>COUNTIFS(consultas[Nº SALA],$M13,consultas[SEXO],N$1)</f>
-        <v>0</v>
+      <c r="N13" t="s">
+        <v>72</v>
       </c>
       <c r="O13">
-        <f>COUNTIFS(consultas[Nº SALA],$M13,consultas[SEXO],O$1)</f>
-        <v>0</v>
+        <f>SUBTOTAL(109,sala_numeros[M])</f>
+        <v>19</v>
       </c>
       <c r="P13">
-        <f>COUNTIF(consultas[Nº SALA],M13)</f>
-        <v>0</v>
+        <f>SUBTOTAL(109,sala_numeros[F])</f>
+        <v>17</v>
+      </c>
+      <c r="Q13">
+        <f>SUBTOTAL(109,sala_numeros[Total])</f>
+        <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -5069,35 +6517,24 @@
       <c r="G14" t="s">
         <v>14</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>4</v>
+      </c>
+      <c r="I14" t="s">
         <v>15</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>16</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>17</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>102</v>
       </c>
-      <c r="M14" t="s">
-        <v>72</v>
-      </c>
-      <c r="N14">
-        <f>SUBTOTAL(109,sala_numeros[M])</f>
-        <v>19</v>
-      </c>
-      <c r="O14">
-        <f>SUBTOTAL(109,sala_numeros[F])</f>
-        <v>17</v>
-      </c>
-      <c r="P14">
-        <f>SUBTOTAL(109,sala_numeros[Total])</f>
-        <v>36</v>
-      </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -5119,20 +6556,24 @@
       <c r="G15" t="s">
         <v>20</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
         <v>31</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>22</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>23</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -5154,20 +6595,24 @@
       <c r="G16" t="s">
         <v>27</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
         <v>15</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>28</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>24</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -5189,20 +6634,24 @@
       <c r="G17" t="s">
         <v>30</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>3</v>
+      </c>
+      <c r="I17" t="s">
         <v>15</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>16</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>17</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -5224,20 +6673,24 @@
       <c r="G18" t="s">
         <v>14</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
         <v>21</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>22</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>23</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -5259,20 +6712,24 @@
       <c r="G19" t="s">
         <v>20</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
         <v>15</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>28</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>24</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -5294,20 +6751,24 @@
       <c r="G20" t="s">
         <v>27</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
         <v>31</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>16</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>17</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -5329,20 +6790,24 @@
       <c r="G21" t="s">
         <v>30</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>3</v>
+      </c>
+      <c r="I21" t="s">
         <v>15</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>22</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>23</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -5364,20 +6829,24 @@
       <c r="G22" t="s">
         <v>14</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>4</v>
+      </c>
+      <c r="I22" t="s">
         <v>21</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>28</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>24</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -5399,20 +6868,24 @@
       <c r="G23" t="s">
         <v>27</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
         <v>21</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>16</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>17</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -5434,20 +6907,24 @@
       <c r="G24" t="s">
         <v>30</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>3</v>
+      </c>
+      <c r="I24" t="s">
         <v>15</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>22</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>23</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -5469,20 +6946,24 @@
       <c r="G25" t="s">
         <v>14</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>4</v>
+      </c>
+      <c r="I25" t="s">
         <v>31</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>28</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>24</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -5504,20 +6985,24 @@
       <c r="G26" t="s">
         <v>20</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
         <v>15</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>16</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>17</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -5539,20 +7024,24 @@
       <c r="G27" t="s">
         <v>27</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>2</v>
+      </c>
+      <c r="I27" t="s">
         <v>15</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>22</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>23</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -5574,20 +7063,24 @@
       <c r="G28" t="s">
         <v>30</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>3</v>
+      </c>
+      <c r="I28" t="s">
         <v>21</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>28</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>24</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -5609,20 +7102,24 @@
       <c r="G29" t="s">
         <v>14</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>4</v>
+      </c>
+      <c r="I29" t="s">
         <v>15</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>16</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>17</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -5644,20 +7141,24 @@
       <c r="G30" t="s">
         <v>20</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
         <v>31</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>22</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>23</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -5679,20 +7180,24 @@
       <c r="G31" t="s">
         <v>27</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>2</v>
+      </c>
+      <c r="I31" t="s">
         <v>15</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>28</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>24</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -5714,20 +7219,24 @@
       <c r="G32" t="s">
         <v>30</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>3</v>
+      </c>
+      <c r="I32" t="s">
         <v>15</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>16</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>17</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -5749,20 +7258,24 @@
       <c r="G33" t="s">
         <v>14</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>4</v>
+      </c>
+      <c r="I33" t="s">
         <v>21</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>22</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>23</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -5784,20 +7297,24 @@
       <c r="G34" t="s">
         <v>20</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
         <v>15</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>28</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>24</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -5819,20 +7336,24 @@
       <c r="G35" t="s">
         <v>27</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>2</v>
+      </c>
+      <c r="I35" t="s">
         <v>31</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>16</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>17</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -5854,20 +7375,24 @@
       <c r="G36" t="s">
         <v>30</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
         <v>15</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>16</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>24</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -5889,30 +7414,46 @@
       <c r="G37" t="s">
         <v>14</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>4</v>
+      </c>
+      <c r="I37" t="s">
         <v>15</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>28</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>23</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="E38" s="2"/>
+      <c r="H38" t="e">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="E39" s="2"/>
+      <c r="H39" t="e">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="E40" s="2"/>
+      <c r="H40" t="e">
+        <f>MATCH(consultas[[#This Row],[EPS]],eps[nombre],0)</f>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -5923,8 +7464,8 @@
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{68DE5A47-6E7D-4191-8B0A-486F24F73547}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{505E8C43-EE5E-4059-9F21-6ABA5F785484}">
-      <formula1>$M$2:$M$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K41:K1048576 J1:J40" xr:uid="{505E8C43-EE5E-4059-9F21-6ABA5F785484}">
+      <formula1>$N$2:$N$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5936,18 +7477,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7662A329-10DC-4280-8EBF-F0ACD8B8D2C9}">
           <x14:formula1>
             <xm:f>Diag.!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H37</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E438D341-FC26-495A-A94E-630E2A99E7E4}">
-          <x14:formula1>
-            <xm:f>EPS!$A$2:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>I1:I37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{08906839-1BF7-4368-9342-684F1E202E83}">
           <x14:formula1>
@@ -5961,7 +7496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E75362-3890-46CF-8427-5C070E9135CC}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -6119,12 +7654,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2260C24-ECBC-4716-8AEF-97E3F62FD32B}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6243,7 +7778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE550DD9-DAE3-4B05-8D11-C395538864D8}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -6349,12 +7884,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4CD760-6740-4E33-90A6-9BF78E4DF061}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6364,8 +7899,8 @@
     <col min="3" max="3" width="6.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="6.85546875" customWidth="1"/>
     <col min="10" max="11" width="9.7109375" customWidth="1"/>
@@ -6421,97 +7956,143 @@
       <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" t="s">
-        <v>71</v>
+      <c r="A3" s="8">
+        <f>MATCH(condiciones[[#Headers],[PACIENTE]],consultas[#Headers],0)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <f>MATCH(condiciones[[#Headers],[FECHA ENTRADA]],consultas[#Headers],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="8">
+        <f>MATCH(condiciones[[#Headers],[SEXO]],consultas[#Headers],0)</f>
+        <v>3</v>
+      </c>
+      <c r="D3" s="8">
+        <f>MATCH(condiciones[[#Headers],[EDAD]],consultas[#Headers],0)</f>
+        <v>4</v>
+      </c>
+      <c r="E3" s="8">
+        <f>MATCH(condiciones[[#Headers],[VALOR CONSULTA]],consultas[#Headers],0)</f>
+        <v>5</v>
+      </c>
+      <c r="F3" s="8">
+        <f>MATCH(condiciones[[#Headers],[SINTOMAS]],consultas[#Headers],0)</f>
+        <v>6</v>
+      </c>
+      <c r="G3" s="8">
+        <f>MATCH(condiciones[[#Headers],[EPS]],consultas[#Headers],0)</f>
+        <v>7</v>
+      </c>
+      <c r="H3" s="8">
+        <f>MATCH(condiciones[[#Headers],[DIAGNOSTICO]],consultas[#Headers],0)</f>
+        <v>9</v>
+      </c>
+      <c r="I3" s="8">
+        <f>MATCH(condiciones[[#Headers],[SALA]],consultas[#Headers],0)</f>
+        <v>10</v>
+      </c>
+      <c r="J3" s="8">
+        <f>MATCH(condiciones[[#Headers],[MEDICO]],consultas[#Headers],0)</f>
+        <v>11</v>
+      </c>
+      <c r="K3" s="8">
+        <f>MATCH(condiciones[[#Headers],[Nº SALA]],consultas[#Headers],0)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4">
-        <f>DCOUNT('Consultas'!A:K,'Consultas'!E1,A1:K2)</f>
-        <v>36</v>
-      </c>
-      <c r="E4">
-        <f>DCOUNT(consultas[#All],'Consultas'!E1,condiciones[#All])</f>
-        <v>36</v>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="5">
-        <f>DAVERAGE('Consultas'!A:K,'Consultas'!E1,A1:K2)</f>
-        <v>41361.111111111109</v>
-      </c>
-      <c r="E5" s="5">
-        <f>DAVERAGE(consultas[#All],consultas[[#Headers],[VALOR CONSULTA]],condiciones[#All])</f>
-        <v>41361.111111111109</v>
+        <v>62</v>
+      </c>
+      <c r="B5">
+        <f>DCOUNT('Consultas'!A:M,'Consultas'!E1,A1:K2)</f>
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <f>DCOUNT(consultas[#All],'Consultas'!E1,condiciones[#All])</f>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="5">
-        <f>DMAX('Consultas'!A:K,'Consultas'!E1,A1:K2)</f>
-        <v>75000</v>
+        <f>DAVERAGE('Consultas'!A:M,'Consultas'!E1,A1:K2)</f>
+        <v>41361.111111111109</v>
       </c>
       <c r="E6" s="5">
-        <f>DMAX(consultas[#All],consultas[[#Headers],[VALOR CONSULTA]],condiciones[#All])</f>
-        <v>75000</v>
+        <f>DAVERAGE(consultas[#All],consultas[[#Headers],[VALOR CONSULTA]],condiciones[#All])</f>
+        <v>41361.111111111109</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="5">
-        <f>DMIN('Consultas'!A:K,'Consultas'!E1,A1:K2)</f>
-        <v>25000</v>
+        <f>DMAX('Consultas'!A:M,'Consultas'!E1,A1:K2)</f>
+        <v>75000</v>
       </c>
       <c r="E7" s="5">
-        <f>DMIN(consultas[#All],consultas[[#Headers],[VALOR CONSULTA]],condiciones[#All])</f>
-        <v>25000</v>
+        <f>DMAX(consultas[#All],consultas[[#Headers],[VALOR CONSULTA]],condiciones[#All])</f>
+        <v>75000</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="5">
+        <f>DMIN('Consultas'!A:M,'Consultas'!E1,A1:K2)</f>
+        <v>25000</v>
+      </c>
+      <c r="E8" s="5">
+        <f>DMIN(consultas[#All],consultas[[#Headers],[VALOR CONSULTA]],condiciones[#All])</f>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="5">
-        <f>DSUM('Consultas'!A:K,'Consultas'!E1,A1:K2)</f>
+      <c r="B9" s="5">
+        <f>DSUM('Consultas'!A:M,'Consultas'!E1,A1:K2)</f>
         <v>1489000</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E9" s="5">
         <f>DSUM(consultas[#All],consultas[[#Headers],[VALOR CONSULTA]],condiciones[#All])</f>
         <v>1489000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>68</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>69</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>